<commit_message>
This version has the numeric columns fixed; pandas column means in the face of na were the issue and the fix was converting to numpy arrays and back
</commit_message>
<xml_diff>
--- a/Trait_field_reconciliation.xlsx
+++ b/Trait_field_reconciliation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanfolk/Documents/GitHub/fagales_traits/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E10D95-1EF6-0445-B3E2-D44B4FAFA67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA169A3D-393F-2C41-842B-30DC61EEC35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="500" windowWidth="27640" windowHeight="16440" activeTab="5" xr2:uid="{C6B1AA54-8E59-A64D-B34D-F6AF41BC593E}"/>
+    <workbookView xWindow="6780" yWindow="500" windowWidth="27640" windowHeight="16440" activeTab="1" xr2:uid="{C6B1AA54-8E59-A64D-B34D-F6AF41BC593E}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2360" uniqueCount="2041">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2395" uniqueCount="2076">
   <si>
     <t>female_flower_part_apex_shape.1.shape</t>
   </si>
@@ -6164,13 +6164,118 @@
   </si>
   <si>
     <t>part_venation.1.part_as_loc</t>
+  </si>
+  <si>
+    <t>leaf position.1</t>
+  </si>
+  <si>
+    <t>article_surface.1</t>
+  </si>
+  <si>
+    <t>article_shape.1</t>
+  </si>
+  <si>
+    <t>phyllichnia_shape.1</t>
+  </si>
+  <si>
+    <t>article_length.1.low</t>
+  </si>
+  <si>
+    <t>article_length.1.high</t>
+  </si>
+  <si>
+    <t>article_width.1.low</t>
+  </si>
+  <si>
+    <t>article_width.1.high</t>
+  </si>
+  <si>
+    <t>branch_position.1</t>
+  </si>
+  <si>
+    <t>branch_length.1.low</t>
+  </si>
+  <si>
+    <t>article_length</t>
+  </si>
+  <si>
+    <t>article_width</t>
+  </si>
+  <si>
+    <t>branch_length</t>
+  </si>
+  <si>
+    <t>article_surface</t>
+  </si>
+  <si>
+    <t>article_shape</t>
+  </si>
+  <si>
+    <t>phyllichnia_shape</t>
+  </si>
+  <si>
+    <t>leaf position</t>
+  </si>
+  <si>
+    <t>branch_position</t>
+  </si>
+  <si>
+    <t>branch_length.1.high</t>
+  </si>
+  <si>
+    <t>leaflet_length</t>
+  </si>
+  <si>
+    <t>leaflet_length.1.low</t>
+  </si>
+  <si>
+    <t>leaflet_length.1.high</t>
+  </si>
+  <si>
+    <t>leaflet_width</t>
+  </si>
+  <si>
+    <t>leaflet_width.1.low</t>
+  </si>
+  <si>
+    <t>leaflet_width.1.high</t>
+  </si>
+  <si>
+    <t>leaflet_number</t>
+  </si>
+  <si>
+    <t>leaflet_number.1.low</t>
+  </si>
+  <si>
+    <t>leaflet_number.1.high</t>
+  </si>
+  <si>
+    <t>fruit_stem_length</t>
+  </si>
+  <si>
+    <t>fruit_stem_length.1.low</t>
+  </si>
+  <si>
+    <t>fruit_stem_length.1.high</t>
+  </si>
+  <si>
+    <t>leaflet_shape</t>
+  </si>
+  <si>
+    <t>leaflet_shape.1</t>
+  </si>
+  <si>
+    <t>fruit_position</t>
+  </si>
+  <si>
+    <t>fruit_position.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6192,6 +6297,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF263238"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -6220,16 +6331,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -6615,13 +6739,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE35713-C632-E740-81C4-585BA25485B0}">
-  <dimension ref="A1:B543"/>
+  <dimension ref="A1:B550"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B523" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A70" sqref="A70"/>
+      <selection pane="bottomRight" activeCell="B542" sqref="B542"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10974,7 +11098,66 @@
         <v>1064</v>
       </c>
     </row>
+    <row r="544" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A544" s="2" t="s">
+        <v>2054</v>
+      </c>
+      <c r="B544" s="2" t="s">
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="545" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A545" s="2" t="s">
+        <v>2055</v>
+      </c>
+      <c r="B545" s="2" t="s">
+        <v>2043</v>
+      </c>
+    </row>
+    <row r="546" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A546" s="2" t="s">
+        <v>2056</v>
+      </c>
+      <c r="B546" s="2" t="s">
+        <v>2044</v>
+      </c>
+    </row>
+    <row r="547" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A547" s="2" t="s">
+        <v>2057</v>
+      </c>
+      <c r="B547" s="4" t="s">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="548" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A548" s="2" t="s">
+        <v>2058</v>
+      </c>
+      <c r="B548" s="2" t="s">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="549" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A549" s="2" t="s">
+        <v>2072</v>
+      </c>
+      <c r="B549" s="2" t="s">
+        <v>2073</v>
+      </c>
+    </row>
+    <row r="550" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A550" s="2" t="s">
+        <v>2074</v>
+      </c>
+      <c r="B550" s="2" t="s">
+        <v>2075</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B547">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -12728,13 +12911,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54B4F97F-35B7-2D49-9600-113A01D012DE}">
-  <dimension ref="A1:F149"/>
+  <dimension ref="A1:F156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B133" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="A153" sqref="A153:D156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14515,6 +14698,90 @@
       </c>
       <c r="D149" t="s">
         <v>1389</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150" s="2" t="s">
+        <v>2051</v>
+      </c>
+      <c r="B150" s="2"/>
+      <c r="C150" s="2" t="s">
+        <v>2045</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>2046</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151" s="2" t="s">
+        <v>2052</v>
+      </c>
+      <c r="B151" s="2"/>
+      <c r="C151" s="2" t="s">
+        <v>2047</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152" s="2" t="s">
+        <v>2053</v>
+      </c>
+      <c r="B152" s="2"/>
+      <c r="C152" s="2" t="s">
+        <v>2050</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>2059</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153" s="2" t="s">
+        <v>2060</v>
+      </c>
+      <c r="B153" s="2"/>
+      <c r="C153" s="2" t="s">
+        <v>2061</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>2062</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154" s="2" t="s">
+        <v>2063</v>
+      </c>
+      <c r="B154" s="2"/>
+      <c r="C154" s="2" t="s">
+        <v>2064</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155" s="2" t="s">
+        <v>2066</v>
+      </c>
+      <c r="B155" s="2"/>
+      <c r="C155" s="2" t="s">
+        <v>2067</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>2068</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156" s="2" t="s">
+        <v>2069</v>
+      </c>
+      <c r="B156" s="2"/>
+      <c r="C156" s="2" t="s">
+        <v>2070</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>2071</v>
       </c>
     </row>
   </sheetData>
@@ -15278,7 +15545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254FCF0D-5DD2-CE4F-81E4-EAD051DBDC93}">
   <dimension ref="A1:A162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A106" sqref="A106:A162"/>
     </sheetView>
   </sheetViews>

</xml_diff>